<commit_message>
Updates R programs and scenarios
</commit_message>
<xml_diff>
--- a/Testing/macro_23_test.xlsx
+++ b/Testing/macro_23_test.xlsx
@@ -223,13 +223,27 @@
       <c r="B11" t="n">
         <v>4.0</v>
       </c>
-      <c r="C11"/>
-      <c r="D11"/>
-      <c r="E11"/>
-      <c r="F11"/>
-      <c r="G11"/>
-      <c r="H11"/>
-      <c r="I11"/>
+      <c r="C11" t="n">
+        <v>0.19508153557370633</v>
+      </c>
+      <c r="D11" t="n">
+        <v>-0.4640841495396</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.6005884338034946</v>
+      </c>
+      <c r="F11" t="n">
+        <v>-0.04700000000000004</v>
+      </c>
+      <c r="G11" t="n">
+        <v>1.5829618029997903</v>
+      </c>
+      <c r="H11" t="n">
+        <v>16.12947350163202</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0.584484590860797</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
@@ -563,13 +577,27 @@
       <c r="B11" t="n">
         <v>4.0</v>
       </c>
-      <c r="C11"/>
-      <c r="D11"/>
-      <c r="E11"/>
-      <c r="F11"/>
-      <c r="G11"/>
-      <c r="H11"/>
-      <c r="I11"/>
+      <c r="C11" t="n">
+        <v>0.19508153557370633</v>
+      </c>
+      <c r="D11" t="n">
+        <v>-0.4640841495396</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.6005884338034946</v>
+      </c>
+      <c r="F11" t="n">
+        <v>-0.04700000000000004</v>
+      </c>
+      <c r="G11" t="n">
+        <v>1.5829618029997903</v>
+      </c>
+      <c r="H11" t="n">
+        <v>16.12947350163202</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0.584484590860797</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="s">

</xml_diff>

<commit_message>
Adds leading quarter to test files
</commit_message>
<xml_diff>
--- a/Testing/macro_23_test.xlsx
+++ b/Testing/macro_23_test.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="17">
   <si>
     <t>Austria</t>
   </si>
@@ -64,18 +64,6 @@
   </si>
   <si>
     <t>RPP</t>
-  </si>
-  <si>
-    <t>2017</t>
-  </si>
-  <si>
-    <t>2018</t>
-  </si>
-  <si>
-    <t>2019</t>
-  </si>
-  <si>
-    <t>2020</t>
   </si>
 </sst>
 </file>
@@ -217,40 +205,26 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="s">
-        <v>17</v>
+      <c r="A11" t="n">
+        <v>2017.0</v>
       </c>
       <c r="B11" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="C11" t="n">
-        <v>0.19508153557370633</v>
-      </c>
-      <c r="D11" t="n">
-        <v>-0.4640841495396</v>
-      </c>
-      <c r="E11" t="n">
-        <v>0.6005884338034946</v>
-      </c>
-      <c r="F11" t="n">
-        <v>-0.04700000000000004</v>
-      </c>
-      <c r="G11" t="n">
-        <v>1.5829618029997903</v>
-      </c>
-      <c r="H11" t="n">
-        <v>16.12947350163202</v>
-      </c>
-      <c r="I11" t="n">
-        <v>0.584484590860797</v>
-      </c>
+        <v>1.0</v>
+      </c>
+      <c r="C11"/>
+      <c r="D11"/>
+      <c r="E11"/>
+      <c r="F11"/>
+      <c r="G11"/>
+      <c r="H11"/>
+      <c r="I11"/>
     </row>
     <row r="12">
-      <c r="A12" t="s">
-        <v>18</v>
+      <c r="A12" t="n">
+        <v>2017.0</v>
       </c>
       <c r="B12" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C12"/>
       <c r="D12"/>
@@ -261,11 +235,11 @@
       <c r="I12"/>
     </row>
     <row r="13">
-      <c r="A13" t="s">
-        <v>18</v>
+      <c r="A13" t="n">
+        <v>2017.0</v>
       </c>
       <c r="B13" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="C13"/>
       <c r="D13"/>
@@ -276,55 +250,55 @@
       <c r="I13"/>
     </row>
     <row r="14">
-      <c r="A14" t="s">
-        <v>18</v>
+      <c r="A14" t="n">
+        <v>2017.0</v>
       </c>
       <c r="B14" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="C14"/>
-      <c r="D14"/>
-      <c r="E14"/>
-      <c r="F14"/>
-      <c r="G14"/>
-      <c r="H14"/>
-      <c r="I14"/>
+        <v>4.0</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.19508153557370633</v>
+      </c>
+      <c r="D14" t="n">
+        <v>-0.4640841495396</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.6005884338034946</v>
+      </c>
+      <c r="F14" t="n">
+        <v>-0.04700000000000004</v>
+      </c>
+      <c r="G14" t="n">
+        <v>1.5829618029997903</v>
+      </c>
+      <c r="H14" t="n">
+        <v>16.12947350163202</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0.584484590860797</v>
+      </c>
     </row>
     <row r="15">
-      <c r="A15" t="s">
-        <v>18</v>
+      <c r="A15" t="n">
+        <v>2018.0</v>
       </c>
       <c r="B15" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="C15" t="n">
-        <v>2.8</v>
-      </c>
-      <c r="D15" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E15" t="n">
-        <v>2.1</v>
-      </c>
-      <c r="F15" t="n">
-        <v>0.09999999999999998</v>
-      </c>
-      <c r="G15" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H15" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="I15" t="n">
-        <v>3.3</v>
-      </c>
+        <v>1.0</v>
+      </c>
+      <c r="C15"/>
+      <c r="D15"/>
+      <c r="E15"/>
+      <c r="F15"/>
+      <c r="G15"/>
+      <c r="H15"/>
+      <c r="I15"/>
     </row>
     <row r="16">
-      <c r="A16" t="s">
-        <v>19</v>
+      <c r="A16" t="n">
+        <v>2018.0</v>
       </c>
       <c r="B16" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C16"/>
       <c r="D16"/>
@@ -335,11 +309,11 @@
       <c r="I16"/>
     </row>
     <row r="17">
-      <c r="A17" t="s">
-        <v>19</v>
+      <c r="A17" t="n">
+        <v>2018.0</v>
       </c>
       <c r="B17" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="C17"/>
       <c r="D17"/>
@@ -350,55 +324,55 @@
       <c r="I17"/>
     </row>
     <row r="18">
-      <c r="A18" t="s">
-        <v>19</v>
+      <c r="A18" t="n">
+        <v>2018.0</v>
       </c>
       <c r="B18" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="C18"/>
-      <c r="D18"/>
-      <c r="E18"/>
-      <c r="F18"/>
-      <c r="G18"/>
-      <c r="H18"/>
-      <c r="I18"/>
+        <v>4.0</v>
+      </c>
+      <c r="C18" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E18" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.09999999999999998</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I18" t="n">
+        <v>3.3</v>
+      </c>
     </row>
     <row r="19">
-      <c r="A19" t="s">
-        <v>19</v>
+      <c r="A19" t="n">
+        <v>2019.0</v>
       </c>
       <c r="B19" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="C19" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="D19" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E19" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="F19" t="n">
-        <v>0.30000000000000004</v>
-      </c>
-      <c r="G19" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H19" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="I19" t="n">
-        <v>3.2</v>
-      </c>
+        <v>1.0</v>
+      </c>
+      <c r="C19"/>
+      <c r="D19"/>
+      <c r="E19"/>
+      <c r="F19"/>
+      <c r="G19"/>
+      <c r="H19"/>
+      <c r="I19"/>
     </row>
     <row r="20">
-      <c r="A20" t="s">
-        <v>20</v>
+      <c r="A20" t="n">
+        <v>2019.0</v>
       </c>
       <c r="B20" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C20"/>
       <c r="D20"/>
@@ -409,11 +383,11 @@
       <c r="I20"/>
     </row>
     <row r="21">
-      <c r="A21" t="s">
-        <v>20</v>
+      <c r="A21" t="n">
+        <v>2019.0</v>
       </c>
       <c r="B21" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="C21"/>
       <c r="D21"/>
@@ -424,46 +398,105 @@
       <c r="I21"/>
     </row>
     <row r="22">
-      <c r="A22" t="s">
-        <v>20</v>
+      <c r="A22" t="n">
+        <v>2019.0</v>
       </c>
       <c r="B22" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C22" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E22" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H22" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I22" t="n">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>2020.0</v>
+      </c>
+      <c r="B23" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C23"/>
+      <c r="D23"/>
+      <c r="E23"/>
+      <c r="F23"/>
+      <c r="G23"/>
+      <c r="H23"/>
+      <c r="I23"/>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>2020.0</v>
+      </c>
+      <c r="B24" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C24"/>
+      <c r="D24"/>
+      <c r="E24"/>
+      <c r="F24"/>
+      <c r="G24"/>
+      <c r="H24"/>
+      <c r="I24"/>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>2020.0</v>
+      </c>
+      <c r="B25" t="n">
         <v>3.0</v>
       </c>
-      <c r="C22"/>
-      <c r="D22"/>
-      <c r="E22"/>
-      <c r="F22"/>
-      <c r="G22"/>
-      <c r="H22"/>
-      <c r="I22"/>
-    </row>
-    <row r="23">
-      <c r="A23" t="s">
-        <v>20</v>
-      </c>
-      <c r="B23" t="n">
+      <c r="C25"/>
+      <c r="D25"/>
+      <c r="E25"/>
+      <c r="F25"/>
+      <c r="G25"/>
+      <c r="H25"/>
+      <c r="I25"/>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>2020.0</v>
+      </c>
+      <c r="B26" t="n">
         <v>4.0</v>
       </c>
-      <c r="C23" t="n">
+      <c r="C26" t="n">
         <v>1.6</v>
       </c>
-      <c r="D23" t="n">
+      <c r="D26" t="n">
         <v>-0.09999999999999964</v>
       </c>
-      <c r="E23" t="n">
+      <c r="E26" t="n">
         <v>1.9</v>
       </c>
-      <c r="F23" t="n">
+      <c r="F26" t="n">
         <v>0.5000000000000001</v>
       </c>
-      <c r="G23" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H23" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="I23" t="n">
+      <c r="G26" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H26" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I26" t="n">
         <v>3.3</v>
       </c>
     </row>
@@ -571,40 +604,26 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="s">
-        <v>17</v>
+      <c r="A11" t="n">
+        <v>2017.0</v>
       </c>
       <c r="B11" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="C11" t="n">
-        <v>0.19508153557370633</v>
-      </c>
-      <c r="D11" t="n">
-        <v>-0.4640841495396</v>
-      </c>
-      <c r="E11" t="n">
-        <v>0.6005884338034946</v>
-      </c>
-      <c r="F11" t="n">
-        <v>-0.04700000000000004</v>
-      </c>
-      <c r="G11" t="n">
-        <v>1.5829618029997903</v>
-      </c>
-      <c r="H11" t="n">
-        <v>16.12947350163202</v>
-      </c>
-      <c r="I11" t="n">
-        <v>0.584484590860797</v>
-      </c>
+        <v>1.0</v>
+      </c>
+      <c r="C11"/>
+      <c r="D11"/>
+      <c r="E11"/>
+      <c r="F11"/>
+      <c r="G11"/>
+      <c r="H11"/>
+      <c r="I11"/>
     </row>
     <row r="12">
-      <c r="A12" t="s">
-        <v>18</v>
+      <c r="A12" t="n">
+        <v>2017.0</v>
       </c>
       <c r="B12" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C12"/>
       <c r="D12"/>
@@ -615,11 +634,11 @@
       <c r="I12"/>
     </row>
     <row r="13">
-      <c r="A13" t="s">
-        <v>18</v>
+      <c r="A13" t="n">
+        <v>2017.0</v>
       </c>
       <c r="B13" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="C13"/>
       <c r="D13"/>
@@ -630,55 +649,55 @@
       <c r="I13"/>
     </row>
     <row r="14">
-      <c r="A14" t="s">
-        <v>18</v>
+      <c r="A14" t="n">
+        <v>2017.0</v>
       </c>
       <c r="B14" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="C14"/>
-      <c r="D14"/>
-      <c r="E14"/>
-      <c r="F14"/>
-      <c r="G14"/>
-      <c r="H14"/>
-      <c r="I14"/>
+        <v>4.0</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.19508153557370633</v>
+      </c>
+      <c r="D14" t="n">
+        <v>-0.4640841495396</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.6005884338034946</v>
+      </c>
+      <c r="F14" t="n">
+        <v>-0.04700000000000004</v>
+      </c>
+      <c r="G14" t="n">
+        <v>1.5829618029997903</v>
+      </c>
+      <c r="H14" t="n">
+        <v>16.12947350163202</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0.584484590860797</v>
+      </c>
     </row>
     <row r="15">
-      <c r="A15" t="s">
-        <v>18</v>
+      <c r="A15" t="n">
+        <v>2018.0</v>
       </c>
       <c r="B15" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="C15" t="n">
-        <v>-1.2</v>
-      </c>
-      <c r="D15" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="E15" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="F15" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="G15" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H15" t="n">
-        <v>-0.6</v>
-      </c>
-      <c r="I15" t="n">
-        <v>-19.1</v>
-      </c>
+        <v>1.0</v>
+      </c>
+      <c r="C15"/>
+      <c r="D15"/>
+      <c r="E15"/>
+      <c r="F15"/>
+      <c r="G15"/>
+      <c r="H15"/>
+      <c r="I15"/>
     </row>
     <row r="16">
-      <c r="A16" t="s">
-        <v>19</v>
+      <c r="A16" t="n">
+        <v>2018.0</v>
       </c>
       <c r="B16" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C16"/>
       <c r="D16"/>
@@ -689,11 +708,11 @@
       <c r="I16"/>
     </row>
     <row r="17">
-      <c r="A17" t="s">
-        <v>19</v>
+      <c r="A17" t="n">
+        <v>2018.0</v>
       </c>
       <c r="B17" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="C17"/>
       <c r="D17"/>
@@ -704,55 +723,55 @@
       <c r="I17"/>
     </row>
     <row r="18">
-      <c r="A18" t="s">
-        <v>19</v>
+      <c r="A18" t="n">
+        <v>2018.0</v>
       </c>
       <c r="B18" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="C18"/>
-      <c r="D18"/>
-      <c r="E18"/>
-      <c r="F18"/>
-      <c r="G18"/>
-      <c r="H18"/>
-      <c r="I18"/>
+        <v>4.0</v>
+      </c>
+      <c r="C18" t="n">
+        <v>-1.2</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E18" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H18" t="n">
+        <v>-0.6</v>
+      </c>
+      <c r="I18" t="n">
+        <v>-19.1</v>
+      </c>
     </row>
     <row r="19">
-      <c r="A19" t="s">
-        <v>19</v>
+      <c r="A19" t="n">
+        <v>2019.0</v>
       </c>
       <c r="B19" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="C19" t="n">
-        <v>-2.5</v>
-      </c>
-      <c r="D19" t="n">
-        <v>1.3000000000000007</v>
-      </c>
-      <c r="E19" t="n">
         <v>1.0</v>
       </c>
-      <c r="F19" t="n">
-        <v>1.1</v>
-      </c>
-      <c r="G19" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H19" t="n">
-        <v>-4.3</v>
-      </c>
-      <c r="I19" t="n">
-        <v>-18.1</v>
-      </c>
+      <c r="C19"/>
+      <c r="D19"/>
+      <c r="E19"/>
+      <c r="F19"/>
+      <c r="G19"/>
+      <c r="H19"/>
+      <c r="I19"/>
     </row>
     <row r="20">
-      <c r="A20" t="s">
-        <v>20</v>
+      <c r="A20" t="n">
+        <v>2019.0</v>
       </c>
       <c r="B20" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C20"/>
       <c r="D20"/>
@@ -763,11 +782,11 @@
       <c r="I20"/>
     </row>
     <row r="21">
-      <c r="A21" t="s">
-        <v>20</v>
+      <c r="A21" t="n">
+        <v>2019.0</v>
       </c>
       <c r="B21" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="C21"/>
       <c r="D21"/>
@@ -778,46 +797,105 @@
       <c r="I21"/>
     </row>
     <row r="22">
-      <c r="A22" t="s">
-        <v>20</v>
+      <c r="A22" t="n">
+        <v>2019.0</v>
       </c>
       <c r="B22" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C22" t="n">
+        <v>-2.5</v>
+      </c>
+      <c r="D22" t="n">
+        <v>1.3000000000000007</v>
+      </c>
+      <c r="E22" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F22" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H22" t="n">
+        <v>-4.3</v>
+      </c>
+      <c r="I22" t="n">
+        <v>-18.1</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>2020.0</v>
+      </c>
+      <c r="B23" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C23"/>
+      <c r="D23"/>
+      <c r="E23"/>
+      <c r="F23"/>
+      <c r="G23"/>
+      <c r="H23"/>
+      <c r="I23"/>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>2020.0</v>
+      </c>
+      <c r="B24" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C24"/>
+      <c r="D24"/>
+      <c r="E24"/>
+      <c r="F24"/>
+      <c r="G24"/>
+      <c r="H24"/>
+      <c r="I24"/>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>2020.0</v>
+      </c>
+      <c r="B25" t="n">
         <v>3.0</v>
       </c>
-      <c r="C22"/>
-      <c r="D22"/>
-      <c r="E22"/>
-      <c r="F22"/>
-      <c r="G22"/>
-      <c r="H22"/>
-      <c r="I22"/>
-    </row>
-    <row r="23">
-      <c r="A23" t="s">
-        <v>20</v>
-      </c>
-      <c r="B23" t="n">
+      <c r="C25"/>
+      <c r="D25"/>
+      <c r="E25"/>
+      <c r="F25"/>
+      <c r="G25"/>
+      <c r="H25"/>
+      <c r="I25"/>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>2020.0</v>
+      </c>
+      <c r="B26" t="n">
         <v>4.0</v>
       </c>
-      <c r="C23" t="n">
+      <c r="C26" t="n">
         <v>0.9</v>
       </c>
-      <c r="D23" t="n">
+      <c r="D26" t="n">
         <v>2.0</v>
       </c>
-      <c r="E23" t="n">
+      <c r="E26" t="n">
         <v>0.7</v>
       </c>
-      <c r="F23" t="n">
+      <c r="F26" t="n">
         <v>1.2999999999999998</v>
       </c>
-      <c r="G23" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H23" t="n">
+      <c r="G26" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H26" t="n">
         <v>-9.9</v>
       </c>
-      <c r="I23" t="n">
+      <c r="I26" t="n">
         <v>0.5</v>
       </c>
     </row>

</xml_diff>